<commit_message>
fixed error on 140-n-max-e test file
</commit_message>
<xml_diff>
--- a/test-files/graph-tests/different-sized-networks/140-genes-0-edges.xlsx
+++ b/test-files/graph-tests/different-sized-networks/140-genes-0-edges.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="60" windowWidth="25140" windowHeight="14120"/>
+    <workbookView xWindow="460" yWindow="60" windowWidth="25100" windowHeight="14120"/>
   </bookViews>
   <sheets>
     <sheet name="network" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="507">
   <si>
     <t>FLO9</t>
   </si>
@@ -1539,6 +1539,9 @@
   <si>
     <t>DAHL</t>
   </si>
+  <si>
+    <t>DUP</t>
+  </si>
 </sst>
 </file>
 
@@ -2470,8 +2473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EK141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DG1" workbookViewId="0">
-      <selection activeCell="DW10" sqref="DW10"/>
+    <sheetView tabSelected="1" topLeftCell="EA1" workbookViewId="0">
+      <selection activeCell="EF1" sqref="EF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2883,7 +2886,7 @@
         <v>498</v>
       </c>
       <c r="EF1" t="s">
-        <v>45</v>
+        <v>506</v>
       </c>
       <c r="EG1" t="s">
         <v>499</v>
@@ -59853,7 +59856,7 @@
     </row>
     <row r="136" spans="1:141">
       <c r="A136" t="s">
-        <v>45</v>
+        <v>506</v>
       </c>
       <c r="B136">
         <v>0</v>

</xml_diff>